<commit_message>
Refactor hero data to actor/character and add game config
Replaces the old hero table with a new actor/character structure, moving hero and enemy data to actor_tbcharacter.json and related C# classes. Introduces game_tbconfig.json and associated classes for game configuration. Updates Tables.cs to use the new structures and reorganizes config and data files accordingly.
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/__tables__.xlsx
+++ b/GameConfigs/Datas/__tables__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\luban_examples-main\MiniTemplate\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ModularSurvivor\GameConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0799C4D2-1E2F-47FB-8D2D-B17421D4963A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494353A6-BB8F-488D-B34F-C4D0CB074DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1035" windowWidth="22785" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>##var</t>
   </si>
@@ -112,6 +112,22 @@
   </si>
   <si>
     <t>reward.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>actor.TbCharacter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Characters</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>目录下包含所有英雄和敌人角色</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -163,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -171,6 +187,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -180,14 +205,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,125 +500,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.375" customWidth="1"/>
     <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="32.375" customWidth="1"/>
+    <col min="4" max="4" width="32.875" customWidth="1"/>
     <col min="5" max="5" width="24.375" customWidth="1"/>
     <col min="6" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="32.125" customWidth="1"/>
+    <col min="13" max="13" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="b">
+      <c r="D4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>